<commit_message>
final commit, finish do an 1
</commit_message>
<xml_diff>
--- a/Giangvien.xlsx
+++ b/Giangvien.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
   <si>
     <t>ma gv</t>
   </si>
@@ -38,202 +38,184 @@
     <t>kinh nghiem gd</t>
   </si>
   <si>
-    <t>GV0001</t>
+    <t>GV0002</t>
+  </si>
+  <si>
+    <t>thinh</t>
+  </si>
+  <si>
+    <t>thinh@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>Thạc sĩ</t>
+  </si>
+  <si>
+    <t>Công nghệ sinh học</t>
+  </si>
+  <si>
+    <t>CNSH</t>
+  </si>
+  <si>
+    <t>2 năm</t>
+  </si>
+  <si>
+    <t>GV0003</t>
+  </si>
+  <si>
+    <t>đợi</t>
+  </si>
+  <si>
+    <t>doi@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>Tiến sĩ</t>
+  </si>
+  <si>
+    <t>Khoa học dữ liệu</t>
+  </si>
+  <si>
+    <t>KHDL</t>
+  </si>
+  <si>
+    <t>3 năm</t>
+  </si>
+  <si>
+    <t>GV0004</t>
+  </si>
+  <si>
+    <t>mộng</t>
+  </si>
+  <si>
+    <t>mong@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>Kĩ sư</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>CNTT</t>
+  </si>
+  <si>
+    <t>4 năm</t>
+  </si>
+  <si>
+    <t>GV0005</t>
+  </si>
+  <si>
+    <t>khoa</t>
+  </si>
+  <si>
+    <t>khoa@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>Kỹ thuật phần mềm</t>
+  </si>
+  <si>
+    <t>KTPM</t>
+  </si>
+  <si>
+    <t>5 năm</t>
+  </si>
+  <si>
+    <t>GV0006</t>
+  </si>
+  <si>
+    <t>lộc</t>
+  </si>
+  <si>
+    <t>loc@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>6 năm</t>
+  </si>
+  <si>
+    <t>GV0007</t>
+  </si>
+  <si>
+    <t>nhựt</t>
+  </si>
+  <si>
+    <t>nhut@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>7 năm</t>
+  </si>
+  <si>
+    <t>GV0009</t>
+  </si>
+  <si>
+    <t>dinh</t>
+  </si>
+  <si>
+    <t>dinh@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>Giáo sư</t>
+  </si>
+  <si>
+    <t>9 năm</t>
+  </si>
+  <si>
+    <t>GV0010</t>
+  </si>
+  <si>
+    <t>bão</t>
+  </si>
+  <si>
+    <t>bao@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>10 năm</t>
+  </si>
+  <si>
+    <t>GV0011</t>
+  </si>
+  <si>
+    <t>lan</t>
+  </si>
+  <si>
+    <t>lan@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>Tân tiến sĩ</t>
+  </si>
+  <si>
+    <t>An ninh mạng</t>
+  </si>
+  <si>
+    <t>ANM</t>
+  </si>
+  <si>
+    <t>11 năm</t>
+  </si>
+  <si>
+    <t>GV0012</t>
+  </si>
+  <si>
+    <t>loan</t>
+  </si>
+  <si>
+    <t>loan@teacher.edu.vn</t>
+  </si>
+  <si>
+    <t>Tân thạc sĩ</t>
+  </si>
+  <si>
+    <t>Luật</t>
+  </si>
+  <si>
+    <t>LUAT</t>
+  </si>
+  <si>
+    <t>12 năm</t>
+  </si>
+  <si>
+    <t>GV00122</t>
   </si>
   <si>
     <t>khang</t>
-  </si>
-  <si>
-    <t>khang@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>Giáo sư</t>
-  </si>
-  <si>
-    <t>Kỹ thuật phần mềm</t>
-  </si>
-  <si>
-    <t>KTPM</t>
-  </si>
-  <si>
-    <t>3 năm</t>
-  </si>
-  <si>
-    <t>GV0002</t>
-  </si>
-  <si>
-    <t>thinh</t>
-  </si>
-  <si>
-    <t>thinh@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>Thạc sĩ</t>
-  </si>
-  <si>
-    <t>Công nghệ sinh học</t>
-  </si>
-  <si>
-    <t>CNSH</t>
-  </si>
-  <si>
-    <t>2 năm</t>
-  </si>
-  <si>
-    <t>GV0003</t>
-  </si>
-  <si>
-    <t>đợi</t>
-  </si>
-  <si>
-    <t>doi@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>Tiến sĩ</t>
-  </si>
-  <si>
-    <t>Khoa học dữ liệu</t>
-  </si>
-  <si>
-    <t>KHDL</t>
-  </si>
-  <si>
-    <t>GV0004</t>
-  </si>
-  <si>
-    <t>mộng</t>
-  </si>
-  <si>
-    <t>mong@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>Kĩ sư</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin</t>
-  </si>
-  <si>
-    <t>CNTT</t>
-  </si>
-  <si>
-    <t>4 năm</t>
-  </si>
-  <si>
-    <t>GV0005</t>
-  </si>
-  <si>
-    <t>khoa</t>
-  </si>
-  <si>
-    <t>khoa@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>5 năm</t>
-  </si>
-  <si>
-    <t>GV0006</t>
-  </si>
-  <si>
-    <t>lộc</t>
-  </si>
-  <si>
-    <t>loc@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>6 năm</t>
-  </si>
-  <si>
-    <t>GV0007</t>
-  </si>
-  <si>
-    <t>nhựt</t>
-  </si>
-  <si>
-    <t>nhut@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>7 năm</t>
-  </si>
-  <si>
-    <t>GV0008</t>
-  </si>
-  <si>
-    <t>nhật</t>
-  </si>
-  <si>
-    <t>nhat@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>8 năm</t>
-  </si>
-  <si>
-    <t>GV0009</t>
-  </si>
-  <si>
-    <t>dinh</t>
-  </si>
-  <si>
-    <t>dinh@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>9 năm</t>
-  </si>
-  <si>
-    <t>GV0010</t>
-  </si>
-  <si>
-    <t>bão</t>
-  </si>
-  <si>
-    <t>bao@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>10 năm</t>
-  </si>
-  <si>
-    <t>GV0011</t>
-  </si>
-  <si>
-    <t>lan</t>
-  </si>
-  <si>
-    <t>lan@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>Tân tiến sĩ</t>
-  </si>
-  <si>
-    <t>An ninh mạng</t>
-  </si>
-  <si>
-    <t>ANM</t>
-  </si>
-  <si>
-    <t>11 năm</t>
-  </si>
-  <si>
-    <t>GV0012</t>
-  </si>
-  <si>
-    <t>loan</t>
-  </si>
-  <si>
-    <t>loan@teacher.edu.vn</t>
-  </si>
-  <si>
-    <t>Tân thạc sĩ</t>
-  </si>
-  <si>
-    <t>Luật</t>
-  </si>
-  <si>
-    <t>LUAT</t>
-  </si>
-  <si>
-    <t>12 năm</t>
-  </si>
-  <si>
-    <t>GV00122</t>
   </si>
   <si>
     <t>abc@teacher.edu.vn</t>
@@ -422,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -446,7 +428,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="n" s="1">
-        <v>40544.0</v>
+        <v>44594.0</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -472,7 +454,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="n" s="1">
-        <v>44594.0</v>
+        <v>44988.0</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -498,7 +480,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="n" s="1">
-        <v>44988.0</v>
+        <v>45386.0</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -513,24 +495,24 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="n" s="1">
-        <v>45386.0</v>
+        <v>42129.0</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
@@ -550,19 +532,19 @@
         <v>36</v>
       </c>
       <c r="C5" t="n" s="1">
-        <v>42129.0</v>
+        <v>42527.0</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
         <v>38</v>
@@ -576,13 +558,13 @@
         <v>40</v>
       </c>
       <c r="C6" t="n" s="1">
-        <v>42527.0</v>
+        <v>44562.0</v>
       </c>
       <c r="D6" t="s">
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -602,221 +584,221 @@
         <v>44</v>
       </c>
       <c r="C7" t="n" s="1">
-        <v>44562.0</v>
+        <v>523821.0</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" t="n" s="1">
-        <v>117642.0</v>
+        <v>45386.0</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" t="n" s="1">
-        <v>523821.0</v>
+        <v>45387.0</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C10" t="n" s="1">
-        <v>45386.0</v>
+        <v>45388.0</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C11" t="n" s="1">
-        <v>45387.0</v>
+        <v>45602.0</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C12" t="n" s="1">
-        <v>45388.0</v>
+        <v>45389.0</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="C13" t="n" s="1">
-        <v>45602.0</v>
+        <v>45390.0</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C14" t="n" s="1">
-        <v>45389.0</v>
+        <v>45391.0</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C15" t="n" s="1">
-        <v>45390.0</v>
+        <v>45392.0</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
         <v>63</v>
@@ -825,76 +807,76 @@
         <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C16" t="n" s="1">
-        <v>45391.0</v>
+        <v>45393.0</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="H16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C17" t="n" s="1">
-        <v>45392.0</v>
+        <v>45394.0</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C18" t="n" s="1">
-        <v>45393.0</v>
+        <v>45395.0</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="F18" t="s">
         <v>63</v>
@@ -903,137 +885,85 @@
         <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C19" t="n" s="1">
-        <v>45394.0</v>
+        <v>45396.0</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C20" t="n" s="1">
-        <v>45395.0</v>
+        <v>45397.0</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" t="s">
         <v>70</v>
-      </c>
-      <c r="G20" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C21" t="n" s="1">
-        <v>45396.0</v>
+        <v>45398.0</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="H21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
         <v>114</v>
-      </c>
-      <c r="B22" t="s">
-        <v>115</v>
-      </c>
-      <c r="C22" t="n" s="1">
-        <v>45397.0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" t="n" s="1">
-        <v>45398.0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>